<commit_message>
added optimal config feature
</commit_message>
<xml_diff>
--- a/src/optimal_config/configurations.xlsx
+++ b/src/optimal_config/configurations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leroytomas\Desktop\GitHub\test_des_sim\src\optimal_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leroytomas\Desktop\GitHub\des_sim-optimal_config\src\optimal_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DACA988-C046-4D78-BBB5-0ED5CD65550B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA33FECC-2CDB-4EDF-B077-E42EC4D91ACF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>chp</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>3-runner</t>
-  </si>
-  <si>
-    <t>4-runner</t>
-  </si>
-  <si>
-    <t>2-runner-dch</t>
   </si>
   <si>
     <t>Air_30kW</t>
@@ -396,32 +390,32 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -429,16 +423,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>50000</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="E2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -446,30 +440,30 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>200</v>
+        <v>200000</v>
       </c>
       <c r="D3">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="E3">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>50000</v>
       </c>
       <c r="D4">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -479,14 +473,8 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -497,7 +485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -511,7 +499,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>

</xml_diff>